<commit_message>
update report no Invoice Plan
</commit_message>
<xml_diff>
--- a/pabi_budget_report/xlsx_template/rpt_budget_future_commit.xlsx
+++ b/pabi_budget_report/xlsx_template/rpt_budget_future_commit.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="90">
   <si>
     <t>Product</t>
   </si>
@@ -299,6 +299,9 @@
   </si>
   <si>
     <t>Subtotal (THB)</t>
+  </si>
+  <si>
+    <t>KV Number</t>
   </si>
 </sst>
 </file>
@@ -797,383 +800,396 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CD13"/>
+  <dimension ref="A1:CE13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="U1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AE14" sqref="AE14"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.7109375" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" customWidth="1"/>
-    <col min="3" max="3" width="21.42578125" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.5703125" customWidth="1"/>
-    <col min="6" max="7" width="20.28515625" customWidth="1"/>
-    <col min="8" max="9" width="15.140625" customWidth="1"/>
-    <col min="10" max="10" width="16.42578125" customWidth="1"/>
-    <col min="11" max="11" width="33.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="29.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16" style="1" customWidth="1"/>
-    <col min="15" max="15" width="19" style="1" customWidth="1"/>
-    <col min="16" max="16" width="15.42578125" style="1" customWidth="1"/>
-    <col min="17" max="17" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12.42578125" customWidth="1"/>
-    <col min="20" max="20" width="13.5703125" customWidth="1"/>
-    <col min="21" max="21" width="11" customWidth="1"/>
-    <col min="22" max="22" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="10" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="13.85546875" customWidth="1"/>
-    <col min="30" max="30" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="17.28515625" customWidth="1"/>
-    <col min="32" max="32" width="9.42578125" customWidth="1"/>
-    <col min="33" max="33" width="16.42578125" customWidth="1"/>
-    <col min="34" max="35" width="12.140625" customWidth="1"/>
-    <col min="36" max="36" width="11" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="13.85546875" customWidth="1"/>
-    <col min="38" max="38" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="16" customWidth="1"/>
-    <col min="40" max="40" width="13.42578125" customWidth="1"/>
-    <col min="41" max="41" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="42" max="44" width="13.85546875" customWidth="1"/>
-    <col min="45" max="45" width="17" customWidth="1"/>
-    <col min="46" max="46" width="18.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="19.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="14" style="5" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="19.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="12.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="13.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="12.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="18.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="23.7109375" style="5" customWidth="1"/>
-    <col min="55" max="55" width="27.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="28.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="12.7109375" style="5" customWidth="1"/>
-    <col min="58" max="58" width="10" style="5" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="10.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="10.5703125" style="5" customWidth="1"/>
-    <col min="61" max="61" width="15.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="62" max="63" width="9.140625" style="5"/>
-    <col min="64" max="64" width="13.7109375" style="5" customWidth="1"/>
-    <col min="65" max="65" width="22.140625" style="5" customWidth="1"/>
-    <col min="66" max="66" width="14.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="18.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="22.42578125" style="5" customWidth="1"/>
-    <col min="69" max="69" width="17.28515625" style="6" customWidth="1"/>
-    <col min="70" max="70" width="11.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="9.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="15.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="73" max="73" width="7" style="6" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="12.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="14.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="76" max="76" width="20.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="77" max="77" width="9.7109375" style="7" customWidth="1"/>
-    <col min="78" max="78" width="14" style="7" bestFit="1" customWidth="1"/>
-    <col min="79" max="79" width="22.42578125" style="7" customWidth="1"/>
-    <col min="80" max="80" width="22" style="7" customWidth="1"/>
+    <col min="1" max="2" width="22.7109375" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" customWidth="1"/>
+    <col min="4" max="4" width="21.42578125" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.5703125" customWidth="1"/>
+    <col min="7" max="8" width="20.28515625" customWidth="1"/>
+    <col min="9" max="10" width="15.140625" customWidth="1"/>
+    <col min="11" max="11" width="16.42578125" customWidth="1"/>
+    <col min="12" max="12" width="33.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="29.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16" style="1" customWidth="1"/>
+    <col min="16" max="16" width="19" style="1" customWidth="1"/>
+    <col min="17" max="17" width="15.42578125" style="1" customWidth="1"/>
+    <col min="18" max="18" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.42578125" customWidth="1"/>
+    <col min="21" max="21" width="13.5703125" customWidth="1"/>
+    <col min="22" max="22" width="11" customWidth="1"/>
+    <col min="23" max="23" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="10" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="13.85546875" customWidth="1"/>
+    <col min="31" max="31" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="17.28515625" customWidth="1"/>
+    <col min="33" max="33" width="9.42578125" customWidth="1"/>
+    <col min="34" max="34" width="16.42578125" customWidth="1"/>
+    <col min="35" max="36" width="12.140625" customWidth="1"/>
+    <col min="37" max="37" width="11" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="13.85546875" customWidth="1"/>
+    <col min="39" max="39" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="16" customWidth="1"/>
+    <col min="41" max="41" width="13.42578125" customWidth="1"/>
+    <col min="42" max="42" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="43" max="45" width="13.85546875" customWidth="1"/>
+    <col min="46" max="46" width="17" customWidth="1"/>
+    <col min="47" max="47" width="18.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="19.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="14" style="5" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="19.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="12.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="13.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="12.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="18.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="23.7109375" style="5" customWidth="1"/>
+    <col min="56" max="56" width="27.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="28.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="12.7109375" style="5" customWidth="1"/>
+    <col min="59" max="59" width="10" style="5" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="10.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="10.5703125" style="5" customWidth="1"/>
+    <col min="62" max="62" width="15.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="63" max="64" width="9.140625" style="5"/>
+    <col min="65" max="65" width="13.7109375" style="5" customWidth="1"/>
+    <col min="66" max="66" width="22.140625" style="5" customWidth="1"/>
+    <col min="67" max="67" width="14.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="18.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="22.42578125" style="5" customWidth="1"/>
+    <col min="70" max="70" width="17.28515625" style="6" customWidth="1"/>
+    <col min="71" max="71" width="11.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="9.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="15.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="7" style="6" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="12.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="14.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="77" max="77" width="20.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="78" max="78" width="9.7109375" style="7" customWidth="1"/>
+    <col min="79" max="79" width="14" style="7" bestFit="1" customWidth="1"/>
+    <col min="80" max="80" width="22.42578125" style="7" customWidth="1"/>
+    <col min="81" max="81" width="22" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:82" ht="15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:83" ht="15" x14ac:dyDescent="0.2">
       <c r="A1" s="20" t="s">
         <v>51</v>
       </c>
+      <c r="B1" s="20"/>
     </row>
-    <row r="2" spans="1:82" ht="15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:83" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="20" t="s">
         <v>50</v>
       </c>
+      <c r="B2" s="20"/>
     </row>
-    <row r="3" spans="1:82" ht="0.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:83" ht="0.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
     </row>
-    <row r="4" spans="1:82" ht="15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:83" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>52</v>
       </c>
+      <c r="B4" s="2"/>
     </row>
-    <row r="5" spans="1:82" ht="15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:83" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="B5" s="2"/>
     </row>
-    <row r="6" spans="1:82" ht="15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:83" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>57</v>
       </c>
+      <c r="B6" s="2"/>
     </row>
-    <row r="7" spans="1:82" ht="15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:83" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>55</v>
       </c>
+      <c r="B7" s="2"/>
     </row>
-    <row r="8" spans="1:82" ht="15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:83" ht="15" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>56</v>
       </c>
+      <c r="B8" s="2"/>
     </row>
-    <row r="9" spans="1:82" ht="15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:83" ht="15" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>53</v>
       </c>
+      <c r="B9" s="3"/>
     </row>
-    <row r="10" spans="1:82" ht="15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:83" ht="15" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>54</v>
       </c>
+      <c r="B10" s="2"/>
     </row>
-    <row r="13" spans="1:82" s="16" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:83" s="16" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="11" t="s">
         <v>49</v>
       </c>
       <c r="B13" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="C13" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="C13" s="11" t="s">
+      <c r="D13" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="D13" s="11" t="s">
+      <c r="E13" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="E13" s="11" t="s">
+      <c r="F13" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="F13" s="11" t="s">
+      <c r="G13" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="G13" s="11" t="s">
+      <c r="H13" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="H13" s="11" t="s">
+      <c r="I13" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="I13" s="11" t="s">
+      <c r="J13" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="J13" s="11" t="s">
+      <c r="K13" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="K13" s="11" t="s">
+      <c r="L13" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="L13" s="8" t="s">
+      <c r="M13" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="M13" s="9" t="s">
+      <c r="N13" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="N13" s="8" t="s">
+      <c r="O13" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="O13" s="8" t="s">
+      <c r="P13" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="P13" s="8" t="s">
+      <c r="Q13" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="Q13" s="9" t="s">
+      <c r="R13" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="R13" s="9" t="s">
+      <c r="S13" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="S13" s="8" t="s">
+      <c r="T13" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="T13" s="8" t="s">
+      <c r="U13" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="U13" s="8" t="s">
+      <c r="V13" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="V13" s="8" t="s">
+      <c r="W13" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="W13" s="8" t="s">
+      <c r="X13" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="X13" s="8" t="s">
+      <c r="Y13" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="Y13" s="8" t="s">
+      <c r="Z13" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="Z13" s="8" t="s">
+      <c r="AA13" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="AA13" s="8" t="s">
+      <c r="AB13" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="AB13" s="8" t="s">
+      <c r="AC13" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="AC13" s="8" t="s">
+      <c r="AD13" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="AD13" s="9" t="s">
+      <c r="AE13" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="AE13" s="9" t="s">
+      <c r="AF13" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="AF13" s="9" t="s">
+      <c r="AG13" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="AG13" s="10" t="s">
+      <c r="AH13" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="AH13" s="10" t="s">
+      <c r="AI13" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="AI13" s="10" t="s">
+      <c r="AJ13" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="AJ13" s="11" t="s">
+      <c r="AK13" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="AK13" s="11" t="s">
+      <c r="AL13" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="AL13" s="11" t="s">
+      <c r="AM13" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="AM13" s="11" t="s">
+      <c r="AN13" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="AN13" s="11" t="s">
+      <c r="AO13" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="AO13" s="11" t="s">
+      <c r="AP13" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="AP13" s="11" t="s">
+      <c r="AQ13" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="AQ13" s="11" t="s">
+      <c r="AR13" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="AR13" s="11" t="s">
+      <c r="AS13" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="AS13" s="11" t="s">
+      <c r="AT13" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="AT13" s="12" t="s">
+      <c r="AU13" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="AU13" s="12" t="s">
+      <c r="AV13" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="AV13" s="12" t="s">
+      <c r="AW13" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="AW13" s="12" t="s">
+      <c r="AX13" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="AX13" s="12" t="s">
+      <c r="AY13" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="AY13" s="12" t="s">
+      <c r="AZ13" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="AZ13" s="12" t="s">
+      <c r="BA13" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="BA13" s="12" t="s">
+      <c r="BB13" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="BB13" s="12" t="s">
+      <c r="BC13" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="BC13" s="12" t="s">
+      <c r="BD13" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="BD13" s="18" t="s">
+      <c r="BE13" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="BE13" s="18" t="s">
+      <c r="BF13" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="BF13" s="18" t="s">
+      <c r="BG13" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="BG13" s="18" t="s">
+      <c r="BH13" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="BH13" s="18" t="s">
+      <c r="BI13" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="BI13" s="18" t="s">
+      <c r="BJ13" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="BJ13" s="19" t="s">
+      <c r="BK13" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="BK13" s="19" t="s">
+      <c r="BL13" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="BL13" s="13" t="s">
+      <c r="BM13" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="BM13" s="13" t="s">
+      <c r="BN13" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="BN13" s="12" t="s">
+      <c r="BO13" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="BO13" s="12" t="s">
+      <c r="BP13" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="BP13" s="12" t="s">
+      <c r="BQ13" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="BQ13" s="14" t="s">
+      <c r="BR13" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="BR13" s="14" t="s">
+      <c r="BS13" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="BS13" s="14" t="s">
+      <c r="BT13" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="BT13" s="14" t="s">
+      <c r="BU13" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="BU13" s="14" t="s">
+      <c r="BV13" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="BV13" s="14" t="s">
+      <c r="BW13" s="14" t="s">
         <v>81</v>
       </c>
-      <c r="BW13" s="14" t="s">
+      <c r="BX13" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="BX13" s="14" t="s">
+      <c r="BY13" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="BY13" s="15" t="s">
+      <c r="BZ13" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="BZ13" s="15" t="s">
+      <c r="CA13" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="CA13" s="15" t="s">
+      <c r="CB13" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="CB13" s="15" t="s">
+      <c r="CC13" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="CC13" s="16" t="s">
+      <c r="CD13" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="CD13" s="17"/>
+      <c r="CE13" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>